<commit_message>
added packages in a single line
</commit_message>
<xml_diff>
--- a/documentation/Cheat Sheet.xlsx
+++ b/documentation/Cheat Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevSRCLocal\UX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevSRCLocal\UX\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87EBF204-661F-4166-98F7-8DEDDF9ED2B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A429783E-4344-4A48-8636-AF2CB79B57F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19710" yWindow="6630" windowWidth="28800" windowHeight="15380" xr2:uid="{FF50B5DF-FD6E-4F78-97D9-8F00F391A731}"/>
+    <workbookView xWindow="5080" yWindow="4330" windowWidth="28800" windowHeight="15380" xr2:uid="{FF50B5DF-FD6E-4F78-97D9-8F00F391A731}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
   <si>
     <t>NT-UX</t>
   </si>
@@ -235,13 +235,22 @@
   </si>
   <si>
     <t>7za</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>updateux</t>
+  </si>
+  <si>
+    <t>update NT-UX to latest version</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,6 +265,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="2">
@@ -284,17 +300,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Encabezado 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Título" xfId="2" builtinId="15"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -606,300 +625,286 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D37562-6B65-486D-B760-306C2A349B04}">
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="20" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" ht="20" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="20" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A6" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>35</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>37</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B8" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>43</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B9" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>38</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>41</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B11" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="20" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="1" t="s">
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="20" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A13" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="14" spans="1:4" ht="20.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A14" t="s">
         <v>45</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B14" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="C14" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>47</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B15" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>48</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B16" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>53</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B17" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>54</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B18" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="C18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>49</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B19" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>50</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B20" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row r="22" spans="1:4" ht="20" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A22" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="20" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>11</v>
-      </c>
-      <c r="B25" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>9</v>
-      </c>
-      <c r="B27" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>65</v>
-      </c>
-      <c r="B30" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="20" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A32" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>15</v>
-      </c>
-      <c r="B33" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>27</v>
-      </c>
-      <c r="B34" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>31</v>
-      </c>
-      <c r="B36" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>33</v>
-      </c>
-      <c r="B37" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="20" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A40" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+    <row r="23" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="C23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C26" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C27" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C29" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Logo and rebranded to System UX
</commit_message>
<xml_diff>
--- a/documentation/Cheat Sheet.xlsx
+++ b/documentation/Cheat Sheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
   <si>
     <t>NT-UX</t>
   </si>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t>create a symbolic link</t>
+  </si>
+  <si>
+    <t>readlink -f link</t>
+  </si>
+  <si>
+    <t>get a symbolic link destination</t>
   </si>
   <si>
     <t>Volumes/File System</t>
@@ -611,7 +617,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -772,98 +778,98 @@
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="25.5">
-      <c r="A14" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="D13" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="2"/>
       <c r="B14" s="2"/>
-      <c r="C14" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="25.5">
+      <c r="A15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="2"/>
+      <c r="C15" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="A16" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="2" t="s">
@@ -875,31 +881,33 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="25.5">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="25.5">
       <c r="A23" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B23" s="2"/>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="3" t="s">
         <v>65</v>
       </c>
       <c r="D23" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
-      <c r="A24" s="2"/>
+      <c r="A24" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D24" s="2"/>
     </row>
@@ -907,7 +915,7 @@
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D25" s="2"/>
     </row>
@@ -915,7 +923,7 @@
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D26" s="2"/>
     </row>
@@ -923,7 +931,7 @@
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D27" s="2"/>
     </row>
@@ -931,7 +939,7 @@
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D28" s="2"/>
     </row>
@@ -939,15 +947,23 @@
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D29" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
+      <c r="C30" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="D30" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>